<commit_message>
En esta nueva versión yse integran las funcionalidades de agregar y eliminar registros, además, interactuan con los saldos de las cuentas
</commit_message>
<xml_diff>
--- a/recursos/validaciones.xlsx
+++ b/recursos/validaciones.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe8c270a4f28cce/Gerardo/9. Proyectos/App finanzas personales/recursos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe8c270a4f28cce/Gerardo/9. Proyectos/App finanzas personales/Github version/Finanzas-personales/recursos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{E9AB1FC4-BCD8-435B-9F6D-3472CD3FAE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88222A32-63B4-434D-B272-EA9AE519E017}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{E9AB1FC4-BCD8-435B-9F6D-3472CD3FAE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11D9B241-68ED-4E80-A4A0-E62C64929907}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{63DBE449-7355-483F-90EB-7FA6CC6C8E2A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>tipo_cuenta</t>
   </si>
@@ -63,6 +63,51 @@
   </si>
   <si>
     <t>Seleccionar…</t>
+  </si>
+  <si>
+    <t>tipo_transaccion</t>
+  </si>
+  <si>
+    <t>Ingreso</t>
+  </si>
+  <si>
+    <t>Gasto</t>
+  </si>
+  <si>
+    <t>categorias</t>
+  </si>
+  <si>
+    <t>Compras</t>
+  </si>
+  <si>
+    <t>Vivienda</t>
+  </si>
+  <si>
+    <t>Transporte</t>
+  </si>
+  <si>
+    <t>Vehículos</t>
+  </si>
+  <si>
+    <t>Vida y entretenimiento</t>
+  </si>
+  <si>
+    <t>Comida y bebida</t>
+  </si>
+  <si>
+    <t>Comunicaciones, PC</t>
+  </si>
+  <si>
+    <t>Gastos financieros</t>
+  </si>
+  <si>
+    <t>Inversiones</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>Transferencia</t>
   </si>
 </sst>
 </file>
@@ -115,10 +160,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -438,57 +479,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B343081A-24E1-4E48-A8C8-9E16D42CE4E8}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>